<commit_message>
delete inputs, now automatic
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2020.xlsx
+++ b/RutaCritica/MallaCurricular2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A5F1C2-0647-4CEB-A84C-8EE78AFEB3CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04C1E32-89CF-4F80-818C-3914B67B221E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="18000" windowHeight="9810" activeTab="2" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2020" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="288">
   <si>
     <t>CBM1000</t>
   </si>
@@ -635,12 +635,6 @@
   </si>
   <si>
     <t>ESTRATEGIAS DE PROGRAMACIÓN</t>
-  </si>
-  <si>
-    <t>CIT3334</t>
-  </si>
-  <si>
-    <t>ESTRUCTURAS DE DATOS COMPACTAS</t>
   </si>
   <si>
     <t>CIT3328</t>
@@ -1130,7 +1124,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{B2ADFDE5-ED7C-4043-8FB7-59A01FC772F5}"/>
   </cellStyles>
@@ -1161,7 +1155,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1459,11 +1453,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1902,7 +1896,7 @@
         <v>75</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>89</v>
@@ -2022,7 +2016,7 @@
         <v>86</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>148</v>
@@ -2143,7 +2137,7 @@
         <v>85</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>87</v>
@@ -2360,7 +2354,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>103</v>
@@ -2400,7 +2394,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>103</v>
@@ -2460,7 +2454,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>103</v>
@@ -2480,7 +2474,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>103</v>
@@ -2500,7 +2494,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>103</v>
@@ -2520,7 +2514,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>103</v>
@@ -2572,7 +2566,7 @@
         <v>11</v>
       </c>
       <c r="F56" s="36" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2583,13 +2577,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F44E877-0DE8-4D93-88A9-15DC654C355E}">
-  <dimension ref="A2:F55"/>
+  <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
@@ -2799,7 +2793,7 @@
         <v>54</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F12" s="40" t="s">
         <v>78</v>
@@ -2926,7 +2920,9 @@
       <c r="D19" s="39">
         <v>54</v>
       </c>
-      <c r="E19" s="38"/>
+      <c r="E19" s="38" t="s">
+        <v>202</v>
+      </c>
       <c r="F19" s="40"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2934,16 +2930,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="39">
+        <v>54</v>
+      </c>
+      <c r="E20" s="38" t="s">
         <v>202</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D20" s="39">
-        <v>54</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>204</v>
       </c>
       <c r="F20" s="40"/>
     </row>
@@ -2961,7 +2957,7 @@
         <v>54</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F21" s="40"/>
     </row>
@@ -2970,16 +2966,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D22" s="39">
         <v>54</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="F22" s="40"/>
     </row>
@@ -2988,54 +2984,54 @@
         <v>1</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="39">
+        <v>54</v>
+      </c>
+      <c r="E23" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="D23" s="39">
-        <v>54</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="40"/>
+      <c r="F23" s="40" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>1</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D24" s="39">
         <v>54</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>110</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="F24" s="40"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>1</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D25" s="39">
         <v>54</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F25" s="40"/>
     </row>
@@ -3044,16 +3040,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D26" s="39">
         <v>54</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>219</v>
+        <v>23</v>
       </c>
       <c r="F26" s="40"/>
     </row>
@@ -3071,7 +3067,7 @@
         <v>54</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>23</v>
+        <v>222</v>
       </c>
       <c r="F27" s="40"/>
     </row>
@@ -3080,16 +3076,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D28" s="39">
         <v>54</v>
       </c>
       <c r="E28" s="38" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F28" s="40"/>
     </row>
@@ -3098,16 +3094,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D29" s="39">
         <v>54</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>228</v>
+        <v>18</v>
       </c>
       <c r="F29" s="40"/>
     </row>
@@ -3125,7 +3121,7 @@
         <v>54</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F30" s="40"/>
     </row>
@@ -3134,16 +3130,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D31" s="39">
         <v>54</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>16</v>
+        <v>222</v>
       </c>
       <c r="F31" s="40"/>
     </row>
@@ -3152,54 +3148,54 @@
         <v>1</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>235</v>
+        <v>156</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>236</v>
+        <v>98</v>
       </c>
       <c r="D32" s="39">
         <v>54</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="F32" s="40"/>
+        <v>23</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>156</v>
+        <v>235</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>98</v>
+        <v>236</v>
       </c>
       <c r="D33" s="39">
         <v>54</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="40" t="s">
-        <v>108</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D34" s="39">
         <v>54</v>
       </c>
       <c r="E34" s="38" t="s">
-        <v>239</v>
+        <v>18</v>
       </c>
       <c r="F34" s="40"/>
     </row>
@@ -3208,10 +3204,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="D35" s="39">
         <v>54</v>
@@ -3226,7 +3222,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>165</v>
+        <v>241</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>242</v>
@@ -3235,25 +3231,25 @@
         <v>54</v>
       </c>
       <c r="E36" s="38" t="s">
-        <v>18</v>
+        <v>243</v>
       </c>
       <c r="F36" s="40"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D37" s="39">
         <v>54</v>
       </c>
       <c r="E37" s="38" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F37" s="40"/>
     </row>
@@ -3262,16 +3258,16 @@
         <v>2</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D38" s="39">
         <v>54</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F38" s="40"/>
     </row>
@@ -3280,16 +3276,16 @@
         <v>2</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D39" s="39">
         <v>54</v>
       </c>
       <c r="E39" s="38" t="s">
-        <v>251</v>
+        <v>22</v>
       </c>
       <c r="F39" s="40"/>
     </row>
@@ -3307,7 +3303,7 @@
         <v>54</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>22</v>
+        <v>254</v>
       </c>
       <c r="F40" s="40"/>
     </row>
@@ -3316,16 +3312,16 @@
         <v>2</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D41" s="39">
         <v>54</v>
       </c>
       <c r="E41" s="38" t="s">
-        <v>256</v>
+        <v>19</v>
       </c>
       <c r="F41" s="40"/>
     </row>
@@ -3343,7 +3339,7 @@
         <v>54</v>
       </c>
       <c r="E42" s="38" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F42" s="40"/>
     </row>
@@ -3361,7 +3357,7 @@
         <v>54</v>
       </c>
       <c r="E43" s="38" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F43" s="40"/>
     </row>
@@ -3379,7 +3375,7 @@
         <v>54</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F44" s="40"/>
     </row>
@@ -3397,7 +3393,7 @@
         <v>54</v>
       </c>
       <c r="E45" s="38" t="s">
-        <v>22</v>
+        <v>249</v>
       </c>
       <c r="F45" s="40"/>
     </row>
@@ -3415,7 +3411,7 @@
         <v>54</v>
       </c>
       <c r="E46" s="38" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F46" s="40"/>
     </row>
@@ -3433,7 +3429,7 @@
         <v>54</v>
       </c>
       <c r="E47" s="38" t="s">
-        <v>248</v>
+        <v>19</v>
       </c>
       <c r="F47" s="40"/>
     </row>
@@ -3451,7 +3447,7 @@
         <v>54</v>
       </c>
       <c r="E48" s="38" t="s">
-        <v>19</v>
+        <v>271</v>
       </c>
       <c r="F48" s="40"/>
     </row>
@@ -3460,16 +3456,16 @@
         <v>2</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D49" s="39">
         <v>54</v>
       </c>
       <c r="E49" s="38" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F49" s="40"/>
     </row>
@@ -3478,16 +3474,16 @@
         <v>2</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D50" s="39">
         <v>54</v>
       </c>
       <c r="E50" s="38" t="s">
-        <v>276</v>
+        <v>22</v>
       </c>
       <c r="F50" s="40"/>
     </row>
@@ -3496,16 +3492,16 @@
         <v>2</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>277</v>
+        <v>231</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>278</v>
+        <v>232</v>
       </c>
       <c r="D51" s="39">
         <v>54</v>
       </c>
       <c r="E51" s="38" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F51" s="40"/>
     </row>
@@ -3514,16 +3510,16 @@
         <v>2</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>233</v>
+        <v>277</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>234</v>
+        <v>278</v>
       </c>
       <c r="D52" s="39">
         <v>54</v>
       </c>
       <c r="E52" s="38" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F52" s="40"/>
     </row>
@@ -3532,56 +3528,38 @@
         <v>2</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>279</v>
+        <v>157</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>280</v>
+        <v>100</v>
       </c>
       <c r="D53" s="39">
         <v>54</v>
       </c>
       <c r="E53" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="F53" s="40"/>
+        <v>19</v>
+      </c>
+      <c r="F53" s="40" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>2</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>157</v>
+        <v>279</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>100</v>
+        <v>280</v>
       </c>
       <c r="D54" s="39">
         <v>54</v>
       </c>
       <c r="E54" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" s="40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="10">
-        <v>2</v>
-      </c>
-      <c r="B55" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="D55" s="39">
-        <v>54</v>
-      </c>
-      <c r="E55" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F55" s="40"/>
+      <c r="F54" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3592,11 +3570,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88EE29A-A5F1-4EDD-B2D2-BD029E8CFEAA}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="49.5703125" customWidth="1"/>

</xml_diff>

<commit_message>
se arreglo los problemas con los excels de la malla 2020
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2020.xlsx
+++ b/RutaCritica/MallaCurricular2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\Protipo TdR - Alfa-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04C1E32-89CF-4F80-818C-3914B67B221E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2F1E2-BE81-4B7F-B4D4-67F7B7556694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="4950" yWindow="3075" windowWidth="18000" windowHeight="9810" activeTab="2" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2020" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="175">
   <si>
     <t>CBM1000</t>
   </si>
@@ -79,36 +79,12 @@
     <t>CBF1002</t>
   </si>
   <si>
-    <t>CIT2001</t>
-  </si>
-  <si>
     <t>CII2750</t>
   </si>
   <si>
-    <t>CIT2002</t>
-  </si>
-  <si>
     <t>CII1000</t>
   </si>
   <si>
-    <t>CIT2005</t>
-  </si>
-  <si>
-    <t>CIT2102</t>
-  </si>
-  <si>
-    <t>CIT2104</t>
-  </si>
-  <si>
-    <t>CIT2004</t>
-  </si>
-  <si>
-    <t>CIT2105</t>
-  </si>
-  <si>
-    <t>CIT2201</t>
-  </si>
-  <si>
     <t>Código</t>
   </si>
   <si>
@@ -499,18 +475,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>CIT3317</t>
-  </si>
-  <si>
-    <t>CIT3346</t>
-  </si>
-  <si>
-    <t>CIT3342</t>
-  </si>
-  <si>
-    <t>CIT3417</t>
-  </si>
-  <si>
     <t>Codigo</t>
   </si>
   <si>
@@ -526,45 +490,9 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>CIT3332</t>
-  </si>
-  <si>
-    <t>ANÁLISIS DE DATOS GEOGRÁFICOS</t>
-  </si>
-  <si>
-    <t>CIT3336</t>
-  </si>
-  <si>
-    <t>CIT3337</t>
-  </si>
-  <si>
-    <t>ASEGURAMIENTO DE CALIDAD</t>
-  </si>
-  <si>
     <t>Equivalencia</t>
   </si>
   <si>
-    <t>BASES DE DATOS DE GRAN VOLUMEN</t>
-  </si>
-  <si>
-    <t>CIT3343</t>
-  </si>
-  <si>
-    <t>BIOINFORMÁTICA</t>
-  </si>
-  <si>
-    <t>CIT3338</t>
-  </si>
-  <si>
-    <t>COMPRESIÓN DE DATOS</t>
-  </si>
-  <si>
-    <t>CIT3320</t>
-  </si>
-  <si>
-    <t>CONTINUIDAD DE NEGOCIOS</t>
-  </si>
-  <si>
     <t>CIT3350</t>
   </si>
   <si>
@@ -574,36 +502,6 @@
     <t>CIT2003, CIT2104, CIT2010, CIT2109</t>
   </si>
   <si>
-    <t>CIT3322</t>
-  </si>
-  <si>
-    <t>DESARROLLO DE APLICACIONES MÓVILES</t>
-  </si>
-  <si>
-    <t>CIT2004, CIT2005</t>
-  </si>
-  <si>
-    <t>CIT3315</t>
-  </si>
-  <si>
-    <t>DESARROLLO DE SOFTWARE DIRIGIDO POR MODE</t>
-  </si>
-  <si>
-    <t>CIT3323</t>
-  </si>
-  <si>
-    <t>DESARROLLO WEB</t>
-  </si>
-  <si>
-    <t>CIT3329</t>
-  </si>
-  <si>
-    <t>DIRECCIÓN Y CONTROL DE PROYECTOS TECNOLÓ</t>
-  </si>
-  <si>
-    <t>CIT1000, CIT2201, CIT2203</t>
-  </si>
-  <si>
     <t>CIT3347</t>
   </si>
   <si>
@@ -613,45 +511,6 @@
     <t>CIT2012, CIT2005</t>
   </si>
   <si>
-    <t>CIT3330</t>
-  </si>
-  <si>
-    <t>DISEÑO DE SISTEMAS TRANSACCIONALES</t>
-  </si>
-  <si>
-    <t>CIT3341</t>
-  </si>
-  <si>
-    <t>E-BUSINESS</t>
-  </si>
-  <si>
-    <t>CIT3331</t>
-  </si>
-  <si>
-    <t>EMPRENDIMIENTO TIC</t>
-  </si>
-  <si>
-    <t>CIT3327</t>
-  </si>
-  <si>
-    <t>ESTRATEGIAS DE PROGRAMACIÓN</t>
-  </si>
-  <si>
-    <t>CIT3328</t>
-  </si>
-  <si>
-    <t>GESTIÓN EN INNOVACIÓN TECNOLÓGICA</t>
-  </si>
-  <si>
-    <t>CIT2201, CIT2203</t>
-  </si>
-  <si>
-    <t>CIT3340</t>
-  </si>
-  <si>
-    <t>GESTION ESTRATÉGICA PARA INFORMÁTICA</t>
-  </si>
-  <si>
     <t>CIT3349</t>
   </si>
   <si>
@@ -661,18 +520,6 @@
     <t>CII2750, CIT2204, CIT2007, CIT2002</t>
   </si>
   <si>
-    <t>CIT3318</t>
-  </si>
-  <si>
-    <t>IMPLEMENTACIÓN DE ALGORITMOS</t>
-  </si>
-  <si>
-    <t>INTELIGENCIA ARTIFICIAL</t>
-  </si>
-  <si>
-    <t>CBM1006, CIT2002, CIT2005, CIT2204</t>
-  </si>
-  <si>
     <t>CIT3325</t>
   </si>
   <si>
@@ -682,66 +529,6 @@
     <t>CIT2005, CIT2012</t>
   </si>
   <si>
-    <t>CIT3335</t>
-  </si>
-  <si>
-    <t>INTERFACE HUMANE MÁQUINA</t>
-  </si>
-  <si>
-    <t>CIT2005, CIT2104</t>
-  </si>
-  <si>
-    <t>CIT3321</t>
-  </si>
-  <si>
-    <t>MINERÍA DE DATOS Y PROCESAMIENTO DE LENG</t>
-  </si>
-  <si>
-    <t>CIT3319</t>
-  </si>
-  <si>
-    <t>MODELOS CENTRADOS EN EL USUARIO</t>
-  </si>
-  <si>
-    <t>CIT2005, CIT2202</t>
-  </si>
-  <si>
-    <t>CIT3344</t>
-  </si>
-  <si>
-    <t>PROC DE DATOS Y TEC DE MACHINE LEARNING</t>
-  </si>
-  <si>
-    <t>CIT2002, CIT2200</t>
-  </si>
-  <si>
-    <t>CIT2002, CIT2202</t>
-  </si>
-  <si>
-    <t>CIT3345</t>
-  </si>
-  <si>
-    <t>PROCESOS ÁGILES</t>
-  </si>
-  <si>
-    <t>CIT3314</t>
-  </si>
-  <si>
-    <t>RECONOCIMIENTO DE PATRONES</t>
-  </si>
-  <si>
-    <t>CIT3414</t>
-  </si>
-  <si>
-    <t>SISTEMA DE ALTA DISPONIBILIDAD</t>
-  </si>
-  <si>
-    <t>CIT3316</t>
-  </si>
-  <si>
-    <t>SISTEMA DE RECOMENDACIÓN</t>
-  </si>
-  <si>
     <t>CIT3348</t>
   </si>
   <si>
@@ -751,138 +538,6 @@
     <t>CIT2005, CIT3100</t>
   </si>
   <si>
-    <t>CIT3339</t>
-  </si>
-  <si>
-    <t>TÉCNICAS AGILES Y AUTOMATICAS PARA PROYE</t>
-  </si>
-  <si>
-    <t>VIDEO JUEGOS</t>
-  </si>
-  <si>
-    <t>CIT3326</t>
-  </si>
-  <si>
-    <t>VISIÓN POR COMPUTADOR</t>
-  </si>
-  <si>
-    <t>CIT2003, CIT2102</t>
-  </si>
-  <si>
-    <t>CIT3425</t>
-  </si>
-  <si>
-    <t>ANÁLISIS Y CONFIG. DE SERVICIOS EN RED</t>
-  </si>
-  <si>
-    <t>CIT2100, CIT2105</t>
-  </si>
-  <si>
-    <t>CIT3426</t>
-  </si>
-  <si>
-    <t>ANÁLISIS Y SIMULACIÓN DE SIST. COMUNIC.</t>
-  </si>
-  <si>
-    <t>CIT2100, CIT2102</t>
-  </si>
-  <si>
-    <t>CIT3424</t>
-  </si>
-  <si>
-    <t>CODIFICACIÓN Y ELEMENTOS DE CRIPTOGRAFÍA</t>
-  </si>
-  <si>
-    <t>CIT3422</t>
-  </si>
-  <si>
-    <t>COMPOSICIÓN MUSICAL ASISTIDA POR COMPUT.</t>
-  </si>
-  <si>
-    <t>CIT2102, CIT2201</t>
-  </si>
-  <si>
-    <t>CIT3421</t>
-  </si>
-  <si>
-    <t>COMUNICACIONES DIGITALES AVANZADAS</t>
-  </si>
-  <si>
-    <t>CIT3427</t>
-  </si>
-  <si>
-    <t>INTERNET DE LAS COSAS</t>
-  </si>
-  <si>
-    <t>CIT3428</t>
-  </si>
-  <si>
-    <t>MÉT. EN DISEÑO DE REDES DE COMUNIC.</t>
-  </si>
-  <si>
-    <t>CIT3416</t>
-  </si>
-  <si>
-    <t>PROCESAMIENTO DIGITAL DE SEÑALES</t>
-  </si>
-  <si>
-    <t>CIT3429</t>
-  </si>
-  <si>
-    <t>PROTOCOLOS DE ENRUTAMIENTO</t>
-  </si>
-  <si>
-    <t>CIT3419</t>
-  </si>
-  <si>
-    <t>REDES DE DATOS AVANZADAS</t>
-  </si>
-  <si>
-    <t>CIT3431</t>
-  </si>
-  <si>
-    <t>REDES MÓVILES CELULARES</t>
-  </si>
-  <si>
-    <t>CIT3420</t>
-  </si>
-  <si>
-    <t>REDES ÓPTICAS DE DATOS</t>
-  </si>
-  <si>
-    <t>CIT2100, CIT2104</t>
-  </si>
-  <si>
-    <t>CIT3430</t>
-  </si>
-  <si>
-    <t>REGULACIÓN DE TICS</t>
-  </si>
-  <si>
-    <t>CIT2102, FIC1003</t>
-  </si>
-  <si>
-    <t>CIT3415</t>
-  </si>
-  <si>
-    <t>SEGURIDAD Y PENTESTING DE APLICACIONES</t>
-  </si>
-  <si>
-    <t>CIT3418</t>
-  </si>
-  <si>
-    <t>SISTEMA EMBEBIDOS</t>
-  </si>
-  <si>
-    <t>CIT3423</t>
-  </si>
-  <si>
-    <t>TELEVISIÓN DIGITAL</t>
-  </si>
-  <si>
-    <t>CIT2102, CIT2200</t>
-  </si>
-  <si>
     <t>INGLÉS GENERAL I</t>
   </si>
   <si>
@@ -899,6 +554,12 @@
   </si>
   <si>
     <t>CIT34XX</t>
+  </si>
+  <si>
+    <t>CIG1003</t>
+  </si>
+  <si>
+    <t>CIG1002</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +695,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1072,13 +733,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1122,9 +796,14 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{B2ADFDE5-ED7C-4043-8FB7-59A01FC772F5}"/>
   </cellStyles>
@@ -1155,7 +834,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1454,10 +1133,10 @@
   <dimension ref="A2:J56"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F35"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1470,22 +1149,22 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1496,16 +1175,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E3" s="21">
         <v>1</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1516,16 +1195,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E4" s="21">
         <v>1</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1536,16 +1215,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E5" s="21">
         <v>1</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1556,16 +1235,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E6" s="21">
         <v>1</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1576,16 +1255,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E7" s="21">
         <v>1</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1596,16 +1275,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E8" s="22">
         <v>2</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1616,16 +1295,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E9" s="22">
         <v>2</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1636,16 +1315,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E10" s="22">
         <v>2</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1656,16 +1335,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E11" s="22">
         <v>2</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1673,19 +1352,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E12" s="22">
         <v>2</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,16 +1375,16 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E13" s="23">
         <v>3</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1716,16 +1395,16 @@
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E14" s="23">
         <v>3</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1736,16 +1415,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E15" s="23">
         <v>3</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1753,19 +1432,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E16" s="23">
         <v>3</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1773,19 +1452,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E17" s="23">
         <v>3</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1796,16 +1475,16 @@
         <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E18" s="24">
         <v>4</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1813,19 +1492,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E19" s="24">
         <v>4</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1836,16 +1515,16 @@
         <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E20" s="24">
         <v>4</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1853,19 +1532,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E21" s="24">
         <v>4</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1873,19 +1552,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E22" s="24">
         <v>4</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1893,19 +1572,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>282</v>
+        <v>167</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E23" s="24">
         <v>4</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1913,19 +1592,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E24" s="25">
         <v>5</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1933,19 +1612,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E25" s="25">
         <v>5</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1953,19 +1632,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E26" s="25">
         <v>5</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1973,19 +1652,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E27" s="25">
         <v>5</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1993,19 +1672,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E28" s="25">
         <v>5</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2013,19 +1692,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>283</v>
+        <v>168</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E29" s="25">
         <v>5</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="J29" s="31"/>
     </row>
@@ -2034,19 +1713,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E30" s="26">
         <v>6</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2054,19 +1733,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E31" s="26">
         <v>6</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2074,19 +1753,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E32" s="26">
         <v>6</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2094,19 +1773,19 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E33" s="26">
         <v>6</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2114,19 +1793,19 @@
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E34" s="26">
         <v>6</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2134,19 +1813,19 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>284</v>
+        <v>169</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E35" s="26">
         <v>6</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2154,19 +1833,19 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E36" s="27">
         <v>7</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2174,19 +1853,19 @@
         <v>35</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E37" s="27">
         <v>7</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2194,19 +1873,19 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E38" s="27">
         <v>7</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2214,19 +1893,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E39" s="27">
         <v>7</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2234,19 +1913,19 @@
         <v>38</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E40" s="27">
         <v>7</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2254,19 +1933,19 @@
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E41" s="28">
         <v>8</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2274,19 +1953,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E42" s="28">
         <v>8</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2294,19 +1973,19 @@
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E43" s="28">
         <v>8</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2314,19 +1993,19 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E44" s="28">
         <v>8</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2334,19 +2013,19 @@
         <v>43</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E45" s="28">
         <v>8</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2354,19 +2033,19 @@
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>286</v>
+        <v>171</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E46" s="29">
         <v>9</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2374,19 +2053,19 @@
         <v>45</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E47" s="29">
         <v>9</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2394,19 +2073,19 @@
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>287</v>
+        <v>172</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E48" s="29">
         <v>9</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2414,19 +2093,19 @@
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E49" s="29">
         <v>9</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2434,19 +2113,19 @@
         <v>48</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E50" s="29">
         <v>9</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2454,19 +2133,19 @@
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>286</v>
+        <v>171</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E51" s="30">
         <v>10</v>
       </c>
       <c r="F51" s="34" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2474,19 +2153,19 @@
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>287</v>
+        <v>172</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E52" s="30">
         <v>10</v>
       </c>
       <c r="F52" s="34" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2494,19 +2173,19 @@
         <v>51</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>287</v>
+        <v>172</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E53" s="30">
         <v>10</v>
       </c>
       <c r="F53" s="34" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2514,19 +2193,19 @@
         <v>52</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>286</v>
+        <v>171</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E54" s="30">
         <v>10</v>
       </c>
       <c r="F54" s="34" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2534,19 +2213,19 @@
         <v>53</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E55" s="30">
         <v>10</v>
       </c>
       <c r="F55" s="34" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2554,19 +2233,19 @@
         <v>54</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E56" s="30">
         <v>11</v>
       </c>
       <c r="F56" s="36" t="s">
-        <v>285</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2577,13 +2256,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F44E877-0DE8-4D93-88A9-15DC654C355E}">
-  <dimension ref="A2:F54"/>
+  <dimension ref="A2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
@@ -2595,22 +2274,22 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2618,16 +2297,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D3" s="39">
         <v>54</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="F3" s="40"/>
     </row>
@@ -2636,16 +2315,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D4" s="39">
         <v>54</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="F4" s="40"/>
     </row>
@@ -2654,36 +2333,34 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D5" s="39">
         <v>54</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>107</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D6" s="39">
         <v>54</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>18</v>
+        <v>163</v>
       </c>
       <c r="F6" s="40"/>
     </row>
@@ -2692,874 +2369,18 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D7" s="39">
         <v>54</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="F7" s="40"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D8" s="39">
-        <v>54</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="40"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9" s="39">
-        <v>54</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="F9" s="40"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="39">
-        <v>54</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="39">
-        <v>54</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="F11" s="40"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>1</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D12" s="39">
-        <v>54</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" s="39">
-        <v>54</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>188</v>
-      </c>
-      <c r="F13" s="40"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>1</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D14" s="39">
-        <v>54</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="F14" s="40"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>1</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" s="39">
-        <v>54</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="40"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>1</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D16" s="39">
-        <v>54</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="40"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>1</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D17" s="39">
-        <v>54</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>1</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D18" s="39">
-        <v>54</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="40"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D19" s="39">
-        <v>54</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="F19" s="40"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D20" s="39">
-        <v>54</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="F20" s="40"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D21" s="39">
-        <v>54</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>207</v>
-      </c>
-      <c r="F21" s="40"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>1</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D22" s="39">
-        <v>54</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="40"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>1</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D23" s="39">
-        <v>54</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="F23" s="40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>1</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D24" s="39">
-        <v>54</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="F24" s="40"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>1</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D25" s="39">
-        <v>54</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="F25" s="40"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>1</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D26" s="39">
-        <v>54</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="40"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>1</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D27" s="39">
-        <v>54</v>
-      </c>
-      <c r="E27" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="F27" s="40"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>1</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D28" s="39">
-        <v>54</v>
-      </c>
-      <c r="E28" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="F28" s="40"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>1</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D29" s="39">
-        <v>54</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="40"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D30" s="39">
-        <v>54</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="40"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="D31" s="39">
-        <v>54</v>
-      </c>
-      <c r="E31" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="F31" s="40"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
-        <v>1</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="39">
-        <v>54</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>1</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="D33" s="39">
-        <v>54</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="F33" s="40"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
-        <v>1</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="D34" s="39">
-        <v>54</v>
-      </c>
-      <c r="E34" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="40"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
-        <v>1</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D35" s="39">
-        <v>54</v>
-      </c>
-      <c r="E35" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="40"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
-        <v>1</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D36" s="39">
-        <v>54</v>
-      </c>
-      <c r="E36" s="38" t="s">
-        <v>243</v>
-      </c>
-      <c r="F36" s="40"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
-        <v>2</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="D37" s="39">
-        <v>54</v>
-      </c>
-      <c r="E37" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="F37" s="40"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
-        <v>2</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="D38" s="39">
-        <v>54</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="F38" s="40"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
-        <v>2</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="D39" s="39">
-        <v>54</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" s="40"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
-        <v>2</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="D40" s="39">
-        <v>54</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="F40" s="40"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
-        <v>2</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D41" s="39">
-        <v>54</v>
-      </c>
-      <c r="E41" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="40"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
-        <v>2</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="39">
-        <v>54</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="40"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
-        <v>2</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="D43" s="39">
-        <v>54</v>
-      </c>
-      <c r="E43" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="40"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
-        <v>2</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D44" s="39">
-        <v>54</v>
-      </c>
-      <c r="E44" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="40"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
-        <v>2</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D45" s="39">
-        <v>54</v>
-      </c>
-      <c r="E45" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="F45" s="40"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="10">
-        <v>2</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="D46" s="39">
-        <v>54</v>
-      </c>
-      <c r="E46" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="F46" s="40"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="10">
-        <v>2</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="D47" s="39">
-        <v>54</v>
-      </c>
-      <c r="E47" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" s="40"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
-        <v>2</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="D48" s="39">
-        <v>54</v>
-      </c>
-      <c r="E48" s="38" t="s">
-        <v>271</v>
-      </c>
-      <c r="F48" s="40"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
-        <v>2</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D49" s="39">
-        <v>54</v>
-      </c>
-      <c r="E49" s="38" t="s">
-        <v>274</v>
-      </c>
-      <c r="F49" s="40"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
-        <v>2</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="D50" s="39">
-        <v>54</v>
-      </c>
-      <c r="E50" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="F50" s="40"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
-        <v>2</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="D51" s="39">
-        <v>54</v>
-      </c>
-      <c r="E51" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" s="40"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
-        <v>2</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="D52" s="39">
-        <v>54</v>
-      </c>
-      <c r="E52" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="40"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="10">
-        <v>2</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D53" s="39">
-        <v>54</v>
-      </c>
-      <c r="E53" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" s="40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="10">
-        <v>2</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D54" s="39">
-        <v>54</v>
-      </c>
-      <c r="E54" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="F54" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3570,11 +2391,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88EE29A-A5F1-4EDD-B2D2-BD029E8CFEAA}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="49.5703125" customWidth="1"/>
@@ -3585,19 +2406,19 @@
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="40">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9">
-        <v>0</v>
+      <c r="A2" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="40">
-        <v>0</v>
-      </c>
-      <c r="B3" s="9">
-        <v>0</v>
+      <c r="A3" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cfg se deben calcular aparte
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2020.xlsx
+++ b/RutaCritica/MallaCurricular2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\Protipo TdR - Alfa-v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2F1E2-BE81-4B7F-B4D4-67F7B7556694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EAEEB3-8CCE-4ED9-9155-7EBF709AAA79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="3075" windowWidth="18000" windowHeight="9810" activeTab="2" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2020" sheetId="1" r:id="rId1"/>
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,7 +2392,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>